<commit_message>
Update input test data
</commit_message>
<xml_diff>
--- a/tests/mjbs_druglist.xlsx
+++ b/tests/mjbs_druglist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasbencomo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasbencomo/code/pharmer/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D608FA-C3C2-9345-AF71-6BCF4E93171F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AB6EA2-1D42-CB47-8CD7-A70F0A8FE8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSK Injuries" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="202">
   <si>
     <t xml:space="preserve">The drugs listed under Prototypes are the ones that will be used for block exam questions. The "Closely related drugs" list contains additional important Immuno drugs that will likely appear in clinical practice.  </t>
   </si>
@@ -152,9 +152,6 @@
   </si>
   <si>
     <t>Methylprenisolone</t>
-  </si>
-  <si>
-    <t>Same as above</t>
   </si>
   <si>
     <t>Administered IV, better bioavailability than oral prednisone</t>
@@ -978,7 +975,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1036,19 +1033,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1266,15 +1250,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -1346,7 +1321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1376,7 +1351,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1385,25 +1360,25 @@
     <xf numFmtId="49" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,7 +1396,25 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1439,25 +1432,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1472,7 +1447,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1481,46 +1456,46 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1538,7 +1513,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1553,13 +1528,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1568,49 +1543,43 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1619,41 +1588,29 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1943,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341A14E4-7829-4DFC-98ED-8BECCF6431C9}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1960,15 +1917,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1999,7 +1956,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="5" customFormat="1" ht="77" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="93" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -2022,7 +1979,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
+      <c r="A5" s="90"/>
       <c r="B5" s="27" t="s">
         <v>15</v>
       </c>
@@ -2057,8 +2014,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="112" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:8" ht="112" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="39" t="s">
@@ -2068,7 +2025,7 @@
       <c r="D7" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="86" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="42" t="s">
@@ -2078,291 +2035,291 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="91"/>
+    <row r="8" spans="1:8" ht="71" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
       <c r="B8" s="66" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="67"/>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="53" t="s">
+    </row>
+    <row r="9" spans="1:8" ht="72" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
+      <c r="B9" s="84" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
-      <c r="B9" s="84" t="s">
+      <c r="C9" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="D9" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="86" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="89" t="s">
+      <c r="G9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="32" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="93" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="89" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="93" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="91" t="s">
+      <c r="B10" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="C10" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="E10" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="F10" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="G10" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="43" t="s">
+    </row>
+    <row r="11" spans="1:8" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="89"/>
+      <c r="B11" s="21" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="91"/>
-      <c r="B11" s="21" t="s">
-        <v>42</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="25" t="s">
+      <c r="G11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="26" t="s">
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="90"/>
+      <c r="B12" s="27" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
-      <c r="B12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="D12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="E12" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="F12" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="G12" s="32" t="s">
         <v>50</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" ht="135" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="C13" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="D13" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="E13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="F13" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="G13" s="38" t="s">
         <v>57</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>58</v>
       </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="C14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="D14" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="E14" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="F14" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="G14" s="38" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="C15" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="D15" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="E15" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="F15" s="37" t="s">
         <v>70</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>71</v>
       </c>
       <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:8" s="7" customFormat="1" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="C16" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="D16" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="E16" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="F16" s="37" t="s">
         <v>76</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>77</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:7" s="8" customFormat="1" ht="41" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="39" t="s">
         <v>78</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>79</v>
       </c>
       <c r="C17" s="45"/>
       <c r="D17" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="F17" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="G17" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="43" t="s">
+    </row>
+    <row r="18" spans="1:7" s="8" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="90"/>
+      <c r="B18" s="27" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="8" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="27" t="s">
-        <v>84</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="31" t="s">
+      <c r="G18" s="48"/>
+    </row>
+    <row r="19" spans="1:7" s="8" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="48"/>
-    </row>
-    <row r="19" spans="1:7" s="8" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="91" t="s">
+      <c r="B19" s="39" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>88</v>
       </c>
       <c r="C19" s="45"/>
       <c r="D19" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="F19" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="G19" s="46"/>
+    </row>
+    <row r="20" spans="1:7" s="8" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="89"/>
+      <c r="B20" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" spans="1:7" s="8" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="91"/>
-      <c r="B20" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="C20" s="49"/>
       <c r="D20" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="F20" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="G20" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="93" t="s">
+    </row>
+    <row r="21" spans="1:7" s="8" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="90"/>
+      <c r="B21" s="27" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="8" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
-      <c r="B21" s="27" t="s">
-        <v>97</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="94"/>
+      <c r="G21" s="92"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -2392,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF1568A-587A-437E-94F8-C91911055CC9}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2409,15 +2366,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2447,55 +2404,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="77" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+    <row r="4" spans="1:8" s="5" customFormat="1" ht="77" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="94" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" ht="77" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="G4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="100"/>
-      <c r="B5" s="21" t="s">
-        <v>103</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>104</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>105</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="77" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="77" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="101"/>
-      <c r="B6" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>29</v>
+        <v>107</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>13</v>
@@ -2503,221 +2464,231 @@
       <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:8" ht="115" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="95" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="40"/>
       <c r="D7" s="41" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" s="42" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="53" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="53" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="96" t="s">
+      <c r="B9" s="66" t="s">
         <v>113</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>114</v>
       </c>
       <c r="C9" s="67"/>
       <c r="D9" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="F9" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="G9" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="53" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="81" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="97"/>
-      <c r="B10" s="27" t="s">
-        <v>119</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="F10" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="64" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="G10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" ht="64" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="96" t="s">
+      <c r="B11" s="60" t="s">
         <v>123</v>
-      </c>
-      <c r="B11" s="60" t="s">
-        <v>124</v>
       </c>
       <c r="C11" s="61"/>
       <c r="D11" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="G11" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="65" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="61" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="96" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
-      <c r="B12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="D12" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="63" t="s">
-        <v>29</v>
+      <c r="E12" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="F12" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="32" t="s">
         <v>127</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="82" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="E13" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="F13" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="G13" s="32" t="s">
         <v>137</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="94" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>139</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>140</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="F14" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="G14" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="32" t="s">
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="96" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" ht="54" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="96" t="s">
+      <c r="B15" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="C15" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="D15" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="E15" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="E15" s="63" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="64" t="s">
+      <c r="G15" s="65"/>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="37" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="96" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="73" t="s">
         <v>149</v>
-      </c>
-      <c r="G15" s="65"/>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="97"/>
-      <c r="B16" s="73" t="s">
-        <v>150</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="83" t="s">
         <v>151</v>
       </c>
-      <c r="E16" s="76" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="83" t="s">
+      <c r="G16" s="53"/>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="96" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="82" t="s">
         <v>152</v>
-      </c>
-      <c r="G16" s="53"/>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="58" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
-      <c r="B17" s="82" t="s">
-        <v>153</v>
       </c>
       <c r="C17" s="78"/>
       <c r="D17" s="77" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="80" t="s">
         <v>154</v>
-      </c>
-      <c r="E17" s="79" t="s">
-        <v>142</v>
-      </c>
-      <c r="F17" s="80" t="s">
-        <v>155</v>
       </c>
       <c r="G17" s="81"/>
       <c r="H17" s="9"/>
@@ -2743,17 +2714,12 @@
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="D24" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A17"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2764,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D416A81-1590-40A1-B143-20817482E945}">
   <dimension ref="A1:H308"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2781,15 +2747,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2824,10 +2790,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>157</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>158</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>24</v>
@@ -2836,170 +2802,174 @@
         <v>25</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="D5" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="E5" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="F5" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="38" t="s">
         <v>165</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="8" customFormat="1" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>167</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>168</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="F6" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" s="8" customFormat="1" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" ht="58" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="102" t="s">
+      <c r="B7" s="15" t="s">
         <v>172</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>173</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="G7" s="20" t="s">
+    </row>
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="58" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
-      <c r="B8" s="27" t="s">
-        <v>178</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="F8" s="31" t="s">
         <v>180</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>181</v>
       </c>
       <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:8" s="8" customFormat="1" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="C9" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="D9" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="E9" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="F9" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="G9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" s="8" customFormat="1" ht="97" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="97" t="s">
         <v>187</v>
       </c>
-      <c r="G9" s="38"/>
-    </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" ht="96" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="102" t="s">
+      <c r="B10" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="C10" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="D10" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="E10" s="69" t="s">
         <v>191</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="F10" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="G10" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="G10" s="59" t="s">
+    </row>
+    <row r="11" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="97" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="103"/>
-      <c r="B11" s="27" t="s">
-        <v>195</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="31" t="s">
         <v>196</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>197</v>
       </c>
       <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:8" s="8" customFormat="1" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>198</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>199</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="F12" s="37" t="s">
+      <c r="G12" s="38" t="s">
         <v>201</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="8" customFormat="1" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -3299,9 +3269,7 @@
     <row r="307" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.2"/>
     <row r="308" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3310,23 +3278,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Final_x0020_Documents_x0020_Received xmlns="ec6d6437-82a3-4562-a260-802073099ba5">false</Final_x0020_Documents_x0020_Received>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001770C2267CD863489E95857CD56567F7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e27cb713ff8ded2892bc7523f10b8af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="47a9570e-0ad9-4c9c-aee8-7e1fdef3a62a" xmlns:ns3="ec6d6437-82a3-4562-a260-802073099ba5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6e59f73b4a689f6ad3bbf39f286790ee" ns2:_="" ns3:_="">
     <xsd:import namespace="47a9570e-0ad9-4c9c-aee8-7e1fdef3a62a"/>
@@ -3555,25 +3506,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD812C7-E9B8-4A84-B5FB-825E9B062FDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Final_x0020_Documents_x0020_Received xmlns="ec6d6437-82a3-4562-a260-802073099ba5">false</Final_x0020_Documents_x0020_Received>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890ED498-97CC-4AAA-B956-EA3464879326}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ec6d6437-82a3-4562-a260-802073099ba5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A1F9026-403C-4402-93D4-3430BE6F4666}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3590,4 +3540,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{890ED498-97CC-4AAA-B956-EA3464879326}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ec6d6437-82a3-4562-a260-802073099ba5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD812C7-E9B8-4A84-B5FB-825E9B062FDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>